<commit_message>
Correccion de la funcion de eliminar y editar de estudiantes y docentes, se remplazaron btn por iconos
</commit_message>
<xml_diff>
--- a/ABCeducando-main/build/web/Doc/documentos/Excel/probandoCargamasiva.xlsx
+++ b/ABCeducando-main/build/web/Doc/documentos/Excel/probandoCargamasiva.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="58">
   <si>
     <t>tarjeta identidad</t>
   </si>
@@ -51,6 +51,153 @@
   </si>
   <si>
     <t>ego.jey@hotmail.com</t>
+  </si>
+  <si>
+    <t>Camilo</t>
+  </si>
+  <si>
+    <t>Nicolas</t>
+  </si>
+  <si>
+    <t>Anthony</t>
+  </si>
+  <si>
+    <t>Kate</t>
+  </si>
+  <si>
+    <t>Yersson</t>
+  </si>
+  <si>
+    <t>Sofia</t>
+  </si>
+  <si>
+    <t>Rosa</t>
+  </si>
+  <si>
+    <t>Eduardo</t>
+  </si>
+  <si>
+    <t>Alejandro</t>
+  </si>
+  <si>
+    <t>Wilmer</t>
+  </si>
+  <si>
+    <t>Leonardo</t>
+  </si>
+  <si>
+    <t>Yura</t>
+  </si>
+  <si>
+    <t>Yisel</t>
+  </si>
+  <si>
+    <t>Jimena</t>
+  </si>
+  <si>
+    <t>Lesly</t>
+  </si>
+  <si>
+    <t>Luz</t>
+  </si>
+  <si>
+    <t>Patricia</t>
+  </si>
+  <si>
+    <t>Jonathan</t>
+  </si>
+  <si>
+    <t>Ortiz</t>
+  </si>
+  <si>
+    <t>Munoz</t>
+  </si>
+  <si>
+    <t>Ramirez</t>
+  </si>
+  <si>
+    <t>Rodriguez</t>
+  </si>
+  <si>
+    <t>Huertas</t>
+  </si>
+  <si>
+    <t>Bustamante</t>
+  </si>
+  <si>
+    <t>Peñaloza</t>
+  </si>
+  <si>
+    <t>Valbuena</t>
+  </si>
+  <si>
+    <t>Puertas</t>
+  </si>
+  <si>
+    <t>Cruz</t>
+  </si>
+  <si>
+    <t>Escudero</t>
+  </si>
+  <si>
+    <t>Remirez</t>
+  </si>
+  <si>
+    <t>Niño</t>
+  </si>
+  <si>
+    <t>Camilo1@gmail.com</t>
+  </si>
+  <si>
+    <t>Nicolas1@gmail.com</t>
+  </si>
+  <si>
+    <t>Anthony1@gmail.com</t>
+  </si>
+  <si>
+    <t>Kate1@gmail.com</t>
+  </si>
+  <si>
+    <t>Yersson1@gmail.com</t>
+  </si>
+  <si>
+    <t>Sofia1@gmail.com</t>
+  </si>
+  <si>
+    <t>Rosa1@gmail.com</t>
+  </si>
+  <si>
+    <t>Eduardo1@gmail.com</t>
+  </si>
+  <si>
+    <t>Alejandro1@gmail.com</t>
+  </si>
+  <si>
+    <t>Wilmer1@gmail.com</t>
+  </si>
+  <si>
+    <t>Leonardo1@gmail.com</t>
+  </si>
+  <si>
+    <t>Yura1@gmail.com</t>
+  </si>
+  <si>
+    <t>Yisel1@gmail.com</t>
+  </si>
+  <si>
+    <t>Jimena1@gmail.com</t>
+  </si>
+  <si>
+    <t>Lesly1@gmail.com</t>
+  </si>
+  <si>
+    <t>Luz1@gmail.com</t>
+  </si>
+  <si>
+    <t>Patricia1@gmail.com</t>
+  </si>
+  <si>
+    <t>Jonathan1@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -382,22 +529,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="14.140625" customWidth="1"/>
     <col min="3" max="3" width="18.42578125" customWidth="1"/>
     <col min="4" max="4" width="18.28515625" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21.28515625" customWidth="1"/>
     <col min="8" max="8" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>1023224321</v>
       </c>
@@ -426,7 +572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1023114123</v>
       </c>
@@ -454,6 +600,546 @@
       <c r="I2" t="s">
         <v>2</v>
       </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1234567897</v>
+      </c>
+      <c r="B3">
+        <v>123456</v>
+      </c>
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3">
+        <v>3226549874</v>
+      </c>
+      <c r="G3" t="s">
+        <v>40</v>
+      </c>
+      <c r="H3" s="1">
+        <v>41116</v>
+      </c>
+      <c r="I3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" s="2"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1234567898</v>
+      </c>
+      <c r="B4">
+        <v>123456</v>
+      </c>
+      <c r="C4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4">
+        <v>3221234567</v>
+      </c>
+      <c r="G4" t="s">
+        <v>41</v>
+      </c>
+      <c r="H4" s="1">
+        <v>41116</v>
+      </c>
+      <c r="I4" t="s">
+        <v>2</v>
+      </c>
+      <c r="J4" s="2"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>1234567899</v>
+      </c>
+      <c r="B5">
+        <v>123456</v>
+      </c>
+      <c r="C5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5">
+        <v>3222136547</v>
+      </c>
+      <c r="G5" t="s">
+        <v>42</v>
+      </c>
+      <c r="H5" s="1">
+        <v>41774</v>
+      </c>
+      <c r="I5" t="s">
+        <v>2</v>
+      </c>
+      <c r="J5" s="2"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>1234567894</v>
+      </c>
+      <c r="B6">
+        <v>123456</v>
+      </c>
+      <c r="C6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6">
+        <v>3179876541</v>
+      </c>
+      <c r="G6" t="s">
+        <v>43</v>
+      </c>
+      <c r="H6" s="1">
+        <v>41774</v>
+      </c>
+      <c r="I6" t="s">
+        <v>2</v>
+      </c>
+      <c r="J6" s="2"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>1234567895</v>
+      </c>
+      <c r="B7">
+        <v>123456</v>
+      </c>
+      <c r="C7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7">
+        <v>3176549872</v>
+      </c>
+      <c r="G7" t="s">
+        <v>44</v>
+      </c>
+      <c r="H7" s="1">
+        <v>41116</v>
+      </c>
+      <c r="I7" t="s">
+        <v>2</v>
+      </c>
+      <c r="J7" s="2"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>1234567896</v>
+      </c>
+      <c r="B8">
+        <v>123456</v>
+      </c>
+      <c r="C8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8">
+        <v>3126547895</v>
+      </c>
+      <c r="G8" t="s">
+        <v>45</v>
+      </c>
+      <c r="H8" s="1">
+        <v>41116</v>
+      </c>
+      <c r="I8" t="s">
+        <v>2</v>
+      </c>
+      <c r="J8" s="2"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>1234567891</v>
+      </c>
+      <c r="B9">
+        <v>123456</v>
+      </c>
+      <c r="C9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9">
+        <v>3216542454</v>
+      </c>
+      <c r="G9" t="s">
+        <v>46</v>
+      </c>
+      <c r="H9" s="1">
+        <v>41774</v>
+      </c>
+      <c r="I9" t="s">
+        <v>2</v>
+      </c>
+      <c r="J9" s="2"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>1234567892</v>
+      </c>
+      <c r="B10">
+        <v>123456</v>
+      </c>
+      <c r="C10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10">
+        <v>3214569874</v>
+      </c>
+      <c r="G10" t="s">
+        <v>47</v>
+      </c>
+      <c r="H10" s="1">
+        <v>41774</v>
+      </c>
+      <c r="I10" t="s">
+        <v>2</v>
+      </c>
+      <c r="J10" s="2"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>1234567893</v>
+      </c>
+      <c r="B11">
+        <v>123456</v>
+      </c>
+      <c r="C11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11">
+        <v>3167985461</v>
+      </c>
+      <c r="G11" t="s">
+        <v>48</v>
+      </c>
+      <c r="H11" s="1">
+        <v>41116</v>
+      </c>
+      <c r="I11" t="s">
+        <v>2</v>
+      </c>
+      <c r="J11" s="2"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>9876543211</v>
+      </c>
+      <c r="B12">
+        <v>123456</v>
+      </c>
+      <c r="C12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" t="s">
+        <v>35</v>
+      </c>
+      <c r="F12">
+        <v>3147985236</v>
+      </c>
+      <c r="G12" t="s">
+        <v>49</v>
+      </c>
+      <c r="H12" s="1">
+        <v>41116</v>
+      </c>
+      <c r="I12" t="s">
+        <v>2</v>
+      </c>
+      <c r="J12" s="2"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>9876543212</v>
+      </c>
+      <c r="B13">
+        <v>123456</v>
+      </c>
+      <c r="C13" t="s">
+        <v>0</v>
+      </c>
+      <c r="D13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" t="s">
+        <v>4</v>
+      </c>
+      <c r="F13">
+        <v>3216542454</v>
+      </c>
+      <c r="G13" t="s">
+        <v>50</v>
+      </c>
+      <c r="H13" s="1">
+        <v>41774</v>
+      </c>
+      <c r="I13" t="s">
+        <v>2</v>
+      </c>
+      <c r="J13" s="2"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>9876543213</v>
+      </c>
+      <c r="B14">
+        <v>123456</v>
+      </c>
+      <c r="C14" t="s">
+        <v>0</v>
+      </c>
+      <c r="D14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" t="s">
+        <v>36</v>
+      </c>
+      <c r="F14">
+        <v>3167985461</v>
+      </c>
+      <c r="G14" t="s">
+        <v>51</v>
+      </c>
+      <c r="H14" s="1">
+        <v>41116</v>
+      </c>
+      <c r="I14" t="s">
+        <v>2</v>
+      </c>
+      <c r="J14" s="2"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>9876543214</v>
+      </c>
+      <c r="B15">
+        <v>123456</v>
+      </c>
+      <c r="C15" t="s">
+        <v>0</v>
+      </c>
+      <c r="D15" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F15">
+        <v>3167985461</v>
+      </c>
+      <c r="G15" t="s">
+        <v>52</v>
+      </c>
+      <c r="H15" s="1">
+        <v>41116</v>
+      </c>
+      <c r="I15" t="s">
+        <v>2</v>
+      </c>
+      <c r="J15" s="2"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>9876543215</v>
+      </c>
+      <c r="B16">
+        <v>123456</v>
+      </c>
+      <c r="C16" t="s">
+        <v>0</v>
+      </c>
+      <c r="D16" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16" t="s">
+        <v>32</v>
+      </c>
+      <c r="F16">
+        <v>3126547895</v>
+      </c>
+      <c r="G16" t="s">
+        <v>53</v>
+      </c>
+      <c r="H16" s="1">
+        <v>41774</v>
+      </c>
+      <c r="I16" t="s">
+        <v>2</v>
+      </c>
+      <c r="J16" s="2"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>9876543216</v>
+      </c>
+      <c r="B17">
+        <v>123456</v>
+      </c>
+      <c r="C17" t="s">
+        <v>0</v>
+      </c>
+      <c r="D17" t="s">
+        <v>23</v>
+      </c>
+      <c r="E17" t="s">
+        <v>38</v>
+      </c>
+      <c r="F17">
+        <v>3216542454</v>
+      </c>
+      <c r="G17" t="s">
+        <v>54</v>
+      </c>
+      <c r="H17" s="1">
+        <v>41116</v>
+      </c>
+      <c r="I17" t="s">
+        <v>2</v>
+      </c>
+      <c r="J17" s="2"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>9876543217</v>
+      </c>
+      <c r="B18">
+        <v>123456</v>
+      </c>
+      <c r="C18" t="s">
+        <v>0</v>
+      </c>
+      <c r="D18" t="s">
+        <v>24</v>
+      </c>
+      <c r="E18" t="s">
+        <v>39</v>
+      </c>
+      <c r="F18">
+        <v>3167985461</v>
+      </c>
+      <c r="G18" t="s">
+        <v>55</v>
+      </c>
+      <c r="H18" s="1">
+        <v>41774</v>
+      </c>
+      <c r="I18" t="s">
+        <v>2</v>
+      </c>
+      <c r="J18" s="2"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>9876543218</v>
+      </c>
+      <c r="B19">
+        <v>123456</v>
+      </c>
+      <c r="C19" t="s">
+        <v>0</v>
+      </c>
+      <c r="D19" t="s">
+        <v>25</v>
+      </c>
+      <c r="E19" t="s">
+        <v>28</v>
+      </c>
+      <c r="F19">
+        <v>3216542454</v>
+      </c>
+      <c r="G19" t="s">
+        <v>56</v>
+      </c>
+      <c r="H19" s="1">
+        <v>41116</v>
+      </c>
+      <c r="I19" t="s">
+        <v>2</v>
+      </c>
+      <c r="J19" s="2"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>9876543219</v>
+      </c>
+      <c r="B20">
+        <v>123456</v>
+      </c>
+      <c r="C20" t="s">
+        <v>0</v>
+      </c>
+      <c r="D20" t="s">
+        <v>26</v>
+      </c>
+      <c r="E20" t="s">
+        <v>27</v>
+      </c>
+      <c r="F20">
+        <v>3167985461</v>
+      </c>
+      <c r="G20" t="s">
+        <v>57</v>
+      </c>
+      <c r="H20" s="1">
+        <v>41774</v>
+      </c>
+      <c r="I20" t="s">
+        <v>2</v>
+      </c>
+      <c r="J20" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>